<commit_message>
Trying to read XLSX files
</commit_message>
<xml_diff>
--- a/data/phase2/legacyData/201811.xlsx
+++ b/data/phase2/legacyData/201811.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellamyphan/Library/Mobile Documents/com~apple~CloudDocs/Money Report/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bellamyphan/IdeaProjects/MoneyApp/data/phase2/legacyData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF27A8-465D-0E4B-8A75-528BD0FAFB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA60A64-F920-9C4B-A1EE-E3C0D1134F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8DDD1AE6-6434-5245-BDCD-F5AA3F01EE9D}"/>
+    <workbookView xWindow="-35760" yWindow="1440" windowWidth="28800" windowHeight="17500" xr2:uid="{8DDD1AE6-6434-5245-BDCD-F5AA3F01EE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,6 +328,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,7 +650,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,6 +693,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="17">
+        <v>43405</v>
+      </c>
       <c r="B2" s="10">
         <v>600.73</v>
       </c>
@@ -708,6 +714,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>43405</v>
+      </c>
       <c r="B3" s="10">
         <v>-37.99</v>
       </c>
@@ -723,6 +732,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>43405</v>
+      </c>
       <c r="B4" s="10">
         <v>-119.95</v>
       </c>

</xml_diff>